<commit_message>
Compiled, ready to send
</commit_message>
<xml_diff>
--- a/cream.xlsx
+++ b/cream.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Наименование</t>
   </si>
   <si>
+    <t xml:space="preserve">Модель</t>
+  </si>
+  <si>
     <t xml:space="preserve">Кол-во</t>
   </si>
   <si>
@@ -34,19 +37,67 @@
     <t xml:space="preserve">Стоимость(руб)</t>
   </si>
   <si>
+    <t xml:space="preserve">Обоснование</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коммутатор</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cisco Switch 2960-24TT</t>
   </si>
   <si>
+    <t xml:space="preserve">Данный коммутатор имеет 24 порта, что позволит расширить сеть без замены сетевого оборудования. Также он является управляемым, что позволяет делать сеть более гибкой.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Маршрутизатор</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cisco RV082</t>
   </si>
   <si>
+    <t xml:space="preserve">Поддержка VPN. Компактный и надёжный.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP — телефон</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cisco IP Phone 7960</t>
   </si>
   <si>
-    <t xml:space="preserve">Патч-корд(1м)</t>
+    <t xml:space="preserve">Отличный телефон Cisco.</t>
   </si>
   <si>
     <t xml:space="preserve">Количество телефонов на каждую комнату</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Патч-корд</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Служит для соединения конечных пользователей с коммутатором. В случае большой удалёности требуется прокладка кабеля внутри помещения с монтажем розеток.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коннектор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RJ-45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коммутаторы отделов требуется соединить с уделёным маршрутизатором. Для этого потребуется прокладка кабеля с обжимом под RJ-45.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кабель</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общая стоимость</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Руб</t>
+  </si>
+  <si>
+    <t xml:space="preserve">И в заключении хочется сказать, что есть много оборудования помимо Cisco, которое так же надёжно, но намного дешевле. Поэтому использовать именно его не обязательно</t>
   </si>
 </sst>
 </file>
@@ -56,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,6 +130,32 @@
     </font>
     <font>
       <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="15"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="32"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -91,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -99,6 +176,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -125,17 +238,53 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -155,7 +304,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
@@ -163,105 +312,191 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.93877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.90816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>40000</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">B2*C2</f>
+      <c r="E2" s="1" t="n">
+        <f aca="false">C2*D2</f>
         <v>160000</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>24000</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">C3*D3</f>
+        <v>24000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <f aca="false">B5*4</f>
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">C4*D4</f>
+        <v>52000</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">C6*D6</f>
+        <v>4800</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>24000</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3*C3</f>
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <f aca="false">B15*4</f>
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>13000</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4*C4</f>
-        <v>52000</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <f aca="false">SUM(10, B15*8, 8)</f>
-        <v>26</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>130</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">B5*C5</f>
-        <v>3380</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="0" t="n">
+      <c r="E7" s="1" t="n">
+        <f aca="false">C7*D7</f>
+        <v>40</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">C8*D8</f>
+        <v>2800</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="9" t="n">
         <f aca="false">SUM(D2:D10)</f>
-        <v>239380</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>1</v>
+        <v>77233</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F7:F8"/>
+  </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B15" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5" type="list">
       <formula1>"1,2,3,4,5,6"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>